<commit_message>
Auto commit 25-05-2025 18:33:35.42
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Core i5 GAMING\Desktop\estimate-drafter\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CE24ACA1-EE6C-4C9B-A373-495F08A6D60B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="130" yWindow="610" windowWidth="18880" windowHeight="6490"/>
+    <workbookView xWindow="135" yWindow="615" windowWidth="18885" windowHeight="6495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimate" sheetId="1" r:id="rId1"/>
@@ -14,13 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
-  <si>
-    <t>Item Name</t>
-  </si>
-  <si>
-    <t>Qty</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Construction of 110mm dia borewell</t>
   </si>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -187,6 +187,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -476,287 +479,279 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B1" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B7" s="1">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+      <c r="B15" s="1">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="1">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+      <c r="B20" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="B21" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+      <c r="B25" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+      <c r="B26" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B26" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="B27" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B29" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="87" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
+      <c r="B32" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="B33" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="1">
         <v>6</v>
       </c>
     </row>

</xml_diff>